<commit_message>
mux axi ip core changed in order to chose pwm freq as integer multiple of the isr freq.
tested on motor testbench with FOC of PMSM
</commit_message>
<xml_diff>
--- a/ip_cores/uz_d_gan_inverter/datasheet/dutycyc_to_temperature.xlsx
+++ b/ip_cores/uz_d_gan_inverter/datasheet/dutycyc_to_temperature.xlsx
@@ -277,11 +277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="721645976"/>
-        <c:axId val="721645584"/>
+        <c:axId val="167997520"/>
+        <c:axId val="167997912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="721645976"/>
+        <c:axId val="167997520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,12 +394,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721645584"/>
+        <c:crossAx val="167997912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="721645584"/>
+        <c:axId val="167997912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +512,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="721645976"/>
+        <c:crossAx val="167997520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1447,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1504,6 +1504,12 @@
         <v>2</v>
       </c>
     </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <f>60*1.6235+20.107</f>
+        <v>117.517</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>